<commit_message>
GESTAOWEB - 6.0 - Correzione report-checklist.xlsx
TESI SPA - GESTAOWEB - 6.0:
Corretto campo "razionale di applicabilità" per test ID 157 nel file report-checklist.xlsx
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111GRUPPOGPI00/TESI_SPA/GESTAOWEB/6.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111GRUPPOGPI00/TESI_SPA/GESTAOWEB/6.0/report-checklist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bugs\FSE2_0\Accreditamento\GESTAOWEB\20240417\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bugs\FSE2_0\Accreditamento\GESTAOWEB\20240527\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2989F571-1141-4D9E-B2CD-81B44E90D5BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82708A20-249D-43D3-8E5C-2B025C1C31D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4613,9 +4613,6 @@
     <t>Questo test non è applicabile perché gli unici valori utilizzabili sono N oppure V.</t>
   </si>
   <si>
-    <t>Questo test non è stato effettuato perché il campo può assumere solo i valori "PROG" oppure "DIR".</t>
-  </si>
-  <si>
     <t>Questo test non è applicabile perché gli unici valori utilizzabili sono quelli riconosciuti.</t>
   </si>
   <si>
@@ -4781,6 +4778,11 @@
   </si>
   <si>
     <t xml:space="preserve"> Il software non gestisce in modo strutturato l'informazione relativa al questo test non è applicabile perché la sezione relativa al quesito diagnostico tale da permetterne l'inserimento nel CDA.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il software non gestisce in modo strutturato le informazioni relative all’osservazione clinica relativa ad un parente biologico che ne consenta poi l'inserimento nella sezione "Storia Clinica" del CDA secondo specifiche.
+Per questo motivo il TEST 11 non può essere eseguito.
+</t>
   </si>
 </sst>
 </file>
@@ -4862,7 +4864,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4879,12 +4881,6 @@
       <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor theme="4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -5128,7 +5124,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5230,9 +5226,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5254,24 +5247,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7734,11 +7709,11 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:T1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="F10" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" ySplit="9" topLeftCell="F164" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="J156" sqref="J156:K159"/>
+      <selection pane="bottomRight" activeCell="L164" sqref="L164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7776,14 +7751,14 @@
       <c r="T1" s="15"/>
     </row>
     <row r="2" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="42" t="s">
+      <c r="B2" s="40"/>
+      <c r="C2" s="41" t="s">
         <v>848</v>
       </c>
-      <c r="D2" s="41"/>
+      <c r="D2" s="40"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -7801,14 +7776,14 @@
       <c r="T2" s="15"/>
     </row>
     <row r="3" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="44"/>
-      <c r="C3" s="49" t="s">
-        <v>871</v>
-      </c>
-      <c r="D3" s="41"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="48" t="s">
+        <v>870</v>
+      </c>
+      <c r="D3" s="40"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -7826,12 +7801,12 @@
       <c r="T3" s="15"/>
     </row>
     <row r="4" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="45"/>
-      <c r="B4" s="46"/>
-      <c r="C4" s="49" t="s">
+      <c r="A4" s="44"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="48" t="s">
         <v>849</v>
       </c>
-      <c r="D4" s="41"/>
+      <c r="D4" s="40"/>
       <c r="E4" s="4"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
@@ -7850,12 +7825,12 @@
       <c r="T4" s="15"/>
     </row>
     <row r="5" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="47"/>
-      <c r="B5" s="48"/>
-      <c r="C5" s="49" t="s">
-        <v>872</v>
-      </c>
-      <c r="D5" s="41"/>
+      <c r="A5" s="46"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="48" t="s">
+        <v>871</v>
+      </c>
+      <c r="D5" s="40"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -7873,8 +7848,8 @@
       <c r="T5" s="15"/>
     </row>
     <row r="6" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="38"/>
-      <c r="B6" s="39"/>
+      <c r="A6" s="37"/>
+      <c r="B6" s="38"/>
       <c r="C6" s="16"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -8993,36 +8968,36 @@
       <c r="E39" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="F39" s="50">
+      <c r="F39" s="23">
         <v>45399</v>
       </c>
-      <c r="G39" s="51" t="s">
-        <v>877</v>
-      </c>
-      <c r="H39" s="51" t="s">
+      <c r="G39" s="24" t="s">
         <v>876</v>
       </c>
-      <c r="I39" s="51" t="s">
-        <v>862</v>
-      </c>
-      <c r="J39" s="52" t="s">
+      <c r="H39" s="24" t="s">
+        <v>875</v>
+      </c>
+      <c r="I39" s="24" t="s">
+        <v>861</v>
+      </c>
+      <c r="J39" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="K39" s="52"/>
-      <c r="L39" s="52" t="s">
+      <c r="K39" s="25"/>
+      <c r="L39" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="M39" s="52" t="s">
+      <c r="M39" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="N39" s="52" t="s">
-        <v>886</v>
-      </c>
-      <c r="O39" s="52" t="s">
+      <c r="N39" s="25" t="s">
+        <v>885</v>
+      </c>
+      <c r="O39" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="P39" s="52" t="s">
-        <v>861</v>
+      <c r="P39" s="25" t="s">
+        <v>860</v>
       </c>
       <c r="Q39" s="25"/>
       <c r="R39" s="26"/>
@@ -9285,41 +9260,41 @@
       <c r="E47" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="F47" s="50">
+      <c r="F47" s="23">
         <v>45399</v>
       </c>
-      <c r="G47" s="51" t="s">
-        <v>879</v>
-      </c>
-      <c r="H47" s="51" t="s">
+      <c r="G47" s="24" t="s">
         <v>878</v>
       </c>
-      <c r="I47" s="51" t="s">
-        <v>862</v>
-      </c>
-      <c r="J47" s="52" t="s">
+      <c r="H47" s="24" t="s">
+        <v>877</v>
+      </c>
+      <c r="I47" s="24" t="s">
+        <v>861</v>
+      </c>
+      <c r="J47" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="K47" s="52"/>
-      <c r="L47" s="52" t="s">
+      <c r="K47" s="25"/>
+      <c r="L47" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="M47" s="52" t="s">
+      <c r="M47" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="N47" s="52" t="s">
-        <v>886</v>
-      </c>
-      <c r="O47" s="52" t="s">
+      <c r="N47" s="25" t="s">
+        <v>885</v>
+      </c>
+      <c r="O47" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="P47" s="52" t="s">
-        <v>861</v>
-      </c>
-      <c r="Q47" s="52"/>
-      <c r="R47" s="53"/>
-      <c r="S47" s="54"/>
-      <c r="T47" s="55" t="s">
+      <c r="P47" s="25" t="s">
+        <v>860</v>
+      </c>
+      <c r="Q47" s="25"/>
+      <c r="R47" s="26"/>
+      <c r="S47" s="36"/>
+      <c r="T47" s="28" t="s">
         <v>104</v>
       </c>
     </row>
@@ -9591,20 +9566,20 @@
       <c r="I55" s="24"/>
       <c r="J55" s="25"/>
       <c r="K55" s="25"/>
-      <c r="L55" s="37" t="s">
+      <c r="L55" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="M55" s="37" t="s">
+      <c r="M55" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="N55" s="37" t="s">
-        <v>886</v>
-      </c>
-      <c r="O55" s="37" t="s">
+      <c r="N55" s="25" t="s">
+        <v>885</v>
+      </c>
+      <c r="O55" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="P55" s="37" t="s">
-        <v>855</v>
+      <c r="P55" s="25" t="s">
+        <v>854</v>
       </c>
       <c r="Q55" s="25"/>
       <c r="R55" s="26"/>
@@ -12975,7 +12950,7 @@
         <v>847</v>
       </c>
       <c r="K154" s="25" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="L154" s="25"/>
       <c r="M154" s="25"/>
@@ -13013,7 +12988,7 @@
         <v>847</v>
       </c>
       <c r="K155" s="25" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="L155" s="25"/>
       <c r="M155" s="25"/>
@@ -13047,11 +13022,11 @@
       <c r="G156" s="24"/>
       <c r="H156" s="24"/>
       <c r="I156" s="24"/>
-      <c r="J156" s="52" t="s">
+      <c r="J156" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K156" s="52" t="s">
-        <v>888</v>
+      <c r="K156" s="25" t="s">
+        <v>887</v>
       </c>
       <c r="L156" s="25"/>
       <c r="M156" s="25"/>
@@ -13085,11 +13060,11 @@
       <c r="G157" s="24"/>
       <c r="H157" s="24"/>
       <c r="I157" s="24"/>
-      <c r="J157" s="52" t="s">
+      <c r="J157" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K157" s="52" t="s">
-        <v>889</v>
+      <c r="K157" s="25" t="s">
+        <v>888</v>
       </c>
       <c r="L157" s="25"/>
       <c r="M157" s="25"/>
@@ -13123,11 +13098,11 @@
       <c r="G158" s="24"/>
       <c r="H158" s="24"/>
       <c r="I158" s="24"/>
-      <c r="J158" s="52" t="s">
+      <c r="J158" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K158" s="52" t="s">
-        <v>864</v>
+      <c r="K158" s="25" t="s">
+        <v>863</v>
       </c>
       <c r="L158" s="25"/>
       <c r="M158" s="25"/>
@@ -13161,11 +13136,11 @@
       <c r="G159" s="24"/>
       <c r="H159" s="24"/>
       <c r="I159" s="24"/>
-      <c r="J159" s="52" t="s">
+      <c r="J159" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K159" s="52" t="s">
-        <v>856</v>
+      <c r="K159" s="25" t="s">
+        <v>855</v>
       </c>
       <c r="L159" s="25"/>
       <c r="M159" s="25"/>
@@ -13199,10 +13174,10 @@
       <c r="G160" s="24"/>
       <c r="H160" s="24"/>
       <c r="I160" s="24"/>
-      <c r="J160" s="52" t="s">
+      <c r="J160" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K160" s="52" t="s">
+      <c r="K160" s="25" t="s">
         <v>850</v>
       </c>
       <c r="L160" s="25"/>
@@ -13237,11 +13212,11 @@
       <c r="G161" s="24"/>
       <c r="H161" s="24"/>
       <c r="I161" s="24"/>
-      <c r="J161" s="52" t="s">
+      <c r="J161" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K161" s="52" t="s">
-        <v>857</v>
+      <c r="K161" s="25" t="s">
+        <v>856</v>
       </c>
       <c r="L161" s="25"/>
       <c r="M161" s="25"/>
@@ -13275,11 +13250,11 @@
       <c r="G162" s="24"/>
       <c r="H162" s="24"/>
       <c r="I162" s="24"/>
-      <c r="J162" s="52" t="s">
+      <c r="J162" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K162" s="52" t="s">
-        <v>858</v>
+      <c r="K162" s="25" t="s">
+        <v>857</v>
       </c>
       <c r="L162" s="25"/>
       <c r="M162" s="25"/>
@@ -13313,11 +13288,11 @@
       <c r="G163" s="24"/>
       <c r="H163" s="24"/>
       <c r="I163" s="24"/>
-      <c r="J163" s="52" t="s">
+      <c r="J163" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K163" s="52" t="s">
-        <v>859</v>
+      <c r="K163" s="25" t="s">
+        <v>858</v>
       </c>
       <c r="L163" s="25"/>
       <c r="M163" s="25"/>
@@ -13351,11 +13326,11 @@
       <c r="G164" s="35"/>
       <c r="H164" s="35"/>
       <c r="I164" s="35"/>
-      <c r="J164" s="52" t="s">
+      <c r="J164" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K164" s="52" t="s">
-        <v>851</v>
+      <c r="K164" s="25" t="s">
+        <v>890</v>
       </c>
       <c r="L164" s="25"/>
       <c r="M164" s="25"/>
@@ -13389,11 +13364,11 @@
       <c r="G165" s="24"/>
       <c r="H165" s="24"/>
       <c r="I165" s="24"/>
-      <c r="J165" s="52" t="s">
+      <c r="J165" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K165" s="52" t="s">
-        <v>852</v>
+      <c r="K165" s="25" t="s">
+        <v>851</v>
       </c>
       <c r="L165" s="25"/>
       <c r="M165" s="25"/>
@@ -13427,11 +13402,11 @@
       <c r="G166" s="24"/>
       <c r="H166" s="24"/>
       <c r="I166" s="24"/>
-      <c r="J166" s="52" t="s">
+      <c r="J166" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K166" s="52" t="s">
-        <v>853</v>
+      <c r="K166" s="25" t="s">
+        <v>852</v>
       </c>
       <c r="L166" s="25"/>
       <c r="M166" s="25"/>
@@ -13461,36 +13436,36 @@
       <c r="E167" s="22" t="s">
         <v>363</v>
       </c>
-      <c r="F167" s="50">
+      <c r="F167" s="23">
         <v>45399</v>
       </c>
-      <c r="G167" s="51" t="s">
+      <c r="G167" s="24" t="s">
+        <v>879</v>
+      </c>
+      <c r="H167" s="24" t="s">
         <v>880</v>
       </c>
-      <c r="H167" s="51" t="s">
+      <c r="I167" s="24" t="s">
         <v>881</v>
       </c>
-      <c r="I167" s="51" t="s">
-        <v>882</v>
-      </c>
-      <c r="J167" s="52" t="s">
+      <c r="J167" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="K167" s="52"/>
-      <c r="L167" s="52" t="s">
+      <c r="K167" s="25"/>
+      <c r="L167" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="M167" s="52" t="s">
+      <c r="M167" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="N167" s="52" t="s">
-        <v>886</v>
-      </c>
-      <c r="O167" s="52" t="s">
+      <c r="N167" s="25" t="s">
+        <v>885</v>
+      </c>
+      <c r="O167" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="P167" s="52" t="s">
-        <v>865</v>
+      <c r="P167" s="25" t="s">
+        <v>864</v>
       </c>
       <c r="Q167" s="25"/>
       <c r="R167" s="26"/>
@@ -13515,36 +13490,36 @@
       <c r="E168" s="22" t="s">
         <v>365</v>
       </c>
-      <c r="F168" s="50">
+      <c r="F168" s="23">
         <v>45399</v>
       </c>
-      <c r="G168" s="51" t="s">
+      <c r="G168" s="24" t="s">
+        <v>882</v>
+      </c>
+      <c r="H168" s="24" t="s">
         <v>883</v>
       </c>
-      <c r="H168" s="51" t="s">
+      <c r="I168" s="24" t="s">
         <v>884</v>
       </c>
-      <c r="I168" s="51" t="s">
+      <c r="J168" s="25" t="s">
+        <v>138</v>
+      </c>
+      <c r="K168" s="25"/>
+      <c r="L168" s="25" t="s">
+        <v>847</v>
+      </c>
+      <c r="M168" s="25" t="s">
+        <v>138</v>
+      </c>
+      <c r="N168" s="25" t="s">
         <v>885</v>
       </c>
-      <c r="J168" s="52" t="s">
+      <c r="O168" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="K168" s="52"/>
-      <c r="L168" s="52" t="s">
-        <v>847</v>
-      </c>
-      <c r="M168" s="52" t="s">
-        <v>138</v>
-      </c>
-      <c r="N168" s="52" t="s">
-        <v>886</v>
-      </c>
-      <c r="O168" s="52" t="s">
-        <v>138</v>
-      </c>
-      <c r="P168" s="52" t="s">
-        <v>865</v>
+      <c r="P168" s="25" t="s">
+        <v>864</v>
       </c>
       <c r="Q168" s="25"/>
       <c r="R168" s="26"/>
@@ -13569,15 +13544,15 @@
       <c r="E169" s="22" t="s">
         <v>367</v>
       </c>
-      <c r="F169" s="50"/>
-      <c r="G169" s="51"/>
-      <c r="H169" s="51"/>
-      <c r="I169" s="51"/>
-      <c r="J169" s="52" t="s">
+      <c r="F169" s="23"/>
+      <c r="G169" s="24"/>
+      <c r="H169" s="24"/>
+      <c r="I169" s="24"/>
+      <c r="J169" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K169" s="52" t="s">
-        <v>890</v>
+      <c r="K169" s="25" t="s">
+        <v>889</v>
       </c>
       <c r="L169" s="25"/>
       <c r="M169" s="25"/>
@@ -13607,15 +13582,15 @@
       <c r="E170" s="22" t="s">
         <v>369</v>
       </c>
-      <c r="F170" s="50"/>
-      <c r="G170" s="51"/>
-      <c r="H170" s="51"/>
-      <c r="I170" s="51"/>
-      <c r="J170" s="52" t="s">
+      <c r="F170" s="23"/>
+      <c r="G170" s="24"/>
+      <c r="H170" s="24"/>
+      <c r="I170" s="24"/>
+      <c r="J170" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K170" s="52" t="s">
-        <v>860</v>
+      <c r="K170" s="25" t="s">
+        <v>859</v>
       </c>
       <c r="L170" s="25"/>
       <c r="M170" s="25"/>
@@ -13645,15 +13620,15 @@
       <c r="E171" s="22" t="s">
         <v>371</v>
       </c>
-      <c r="F171" s="50"/>
-      <c r="G171" s="51"/>
-      <c r="H171" s="51"/>
-      <c r="I171" s="51"/>
-      <c r="J171" s="52" t="s">
+      <c r="F171" s="23"/>
+      <c r="G171" s="24"/>
+      <c r="H171" s="24"/>
+      <c r="I171" s="24"/>
+      <c r="J171" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K171" s="52" t="s">
-        <v>870</v>
+      <c r="K171" s="25" t="s">
+        <v>869</v>
       </c>
       <c r="L171" s="25"/>
       <c r="M171" s="25"/>
@@ -13683,15 +13658,15 @@
       <c r="E172" s="22" t="s">
         <v>373</v>
       </c>
-      <c r="F172" s="50"/>
-      <c r="G172" s="51"/>
-      <c r="H172" s="51"/>
-      <c r="I172" s="51"/>
-      <c r="J172" s="52" t="s">
+      <c r="F172" s="23"/>
+      <c r="G172" s="24"/>
+      <c r="H172" s="24"/>
+      <c r="I172" s="24"/>
+      <c r="J172" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K172" s="52" t="s">
-        <v>869</v>
+      <c r="K172" s="25" t="s">
+        <v>868</v>
       </c>
       <c r="L172" s="25"/>
       <c r="M172" s="25"/>
@@ -13721,15 +13696,15 @@
       <c r="E173" s="22" t="s">
         <v>375</v>
       </c>
-      <c r="F173" s="50"/>
-      <c r="G173" s="51"/>
-      <c r="H173" s="51"/>
-      <c r="I173" s="51"/>
-      <c r="J173" s="52" t="s">
+      <c r="F173" s="23"/>
+      <c r="G173" s="24"/>
+      <c r="H173" s="24"/>
+      <c r="I173" s="24"/>
+      <c r="J173" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K173" s="52" t="s">
-        <v>868</v>
+      <c r="K173" s="25" t="s">
+        <v>867</v>
       </c>
       <c r="L173" s="25"/>
       <c r="M173" s="25"/>
@@ -13759,15 +13734,15 @@
       <c r="E174" s="22" t="s">
         <v>377</v>
       </c>
-      <c r="F174" s="50"/>
-      <c r="G174" s="51"/>
-      <c r="H174" s="51"/>
-      <c r="I174" s="51"/>
-      <c r="J174" s="52" t="s">
+      <c r="F174" s="23"/>
+      <c r="G174" s="24"/>
+      <c r="H174" s="24"/>
+      <c r="I174" s="24"/>
+      <c r="J174" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K174" s="52" t="s">
-        <v>867</v>
+      <c r="K174" s="25" t="s">
+        <v>866</v>
       </c>
       <c r="L174" s="25"/>
       <c r="M174" s="25"/>
@@ -13797,15 +13772,15 @@
       <c r="E175" s="22" t="s">
         <v>379</v>
       </c>
-      <c r="F175" s="50"/>
-      <c r="G175" s="51"/>
-      <c r="H175" s="51"/>
-      <c r="I175" s="51"/>
-      <c r="J175" s="52" t="s">
+      <c r="F175" s="23"/>
+      <c r="G175" s="24"/>
+      <c r="H175" s="24"/>
+      <c r="I175" s="24"/>
+      <c r="J175" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K175" s="52" t="s">
-        <v>866</v>
+      <c r="K175" s="25" t="s">
+        <v>865</v>
       </c>
       <c r="L175" s="25"/>
       <c r="M175" s="25"/>
@@ -13835,15 +13810,15 @@
       <c r="E176" s="22" t="s">
         <v>381</v>
       </c>
-      <c r="F176" s="50"/>
-      <c r="G176" s="51"/>
-      <c r="H176" s="51"/>
-      <c r="I176" s="51"/>
-      <c r="J176" s="52" t="s">
+      <c r="F176" s="23"/>
+      <c r="G176" s="24"/>
+      <c r="H176" s="24"/>
+      <c r="I176" s="24"/>
+      <c r="J176" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K176" s="52" t="s">
-        <v>854</v>
+      <c r="K176" s="25" t="s">
+        <v>853</v>
       </c>
       <c r="L176" s="25"/>
       <c r="M176" s="25"/>
@@ -20809,22 +20784,22 @@
       <c r="E381" s="22" t="s">
         <v>789</v>
       </c>
-      <c r="F381" s="50">
+      <c r="F381" s="23">
         <v>45399</v>
       </c>
-      <c r="G381" s="51" t="s">
+      <c r="G381" s="24" t="s">
+        <v>872</v>
+      </c>
+      <c r="H381" s="24" t="s">
         <v>873</v>
       </c>
-      <c r="H381" s="51" t="s">
+      <c r="I381" s="24" t="s">
         <v>874</v>
       </c>
-      <c r="I381" s="51" t="s">
-        <v>875</v>
-      </c>
-      <c r="J381" s="52" t="s">
+      <c r="J381" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="K381" s="52"/>
+      <c r="K381" s="25"/>
       <c r="L381" s="25"/>
       <c r="M381" s="25"/>
       <c r="N381" s="25"/>

</xml_diff>